<commit_message>
Fix question analysis display and Excel processing for Mathematics CT 2
Excel Processing Fixes:
- Fix regex pattern to properly parse "1 Top Ten Questions Skipped/Wrong" headers
- Section 1 now correctly shows mostSkipped and mostWrong data (10 questions each)

Question Analysis Display Fixes:
- Only show sections with actual data (hide empty sections 2 & 3)
- Show ALL questions in each category instead of limiting to first 5
- Add scrollable containers (max-h-64) for better UX with longer lists
- Fix dynamic question ID formatting for any section number
- Update latest Excel data with corrected mostSkipped/mostWrong parsing

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Results/Mathematics CT 2.xlsx
+++ b/Results/Mathematics CT 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\results giver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VH Website\vh-website\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AF308F-A5C6-4305-9D08-E84120E2FEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFC3420-8656-4CE5-AEF6-564B61D1EF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView zoomScale="68" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22:W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1118,7 +1118,7 @@
       </c>
       <c r="W2">
         <f t="shared" ref="W2:W22" si="6">_xlfn.RANK.EQ(V2, $V$2:$V$1000, 0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X2" t="s">
         <v>13</v>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="W3">
         <f t="shared" si="6"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="X3" t="s">
         <v>15</v>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="W4">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y4">
         <f>SUM(Y1:Y3)</f>
@@ -1260,7 +1260,7 @@
       </c>
       <c r="W5">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1306,7 +1306,7 @@
       </c>
       <c r="W6">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Y6" t="s">
         <v>19</v>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="W7">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="W8">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="W9">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1484,7 +1484,7 @@
       </c>
       <c r="W10">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1524,7 +1524,7 @@
       </c>
       <c r="W11">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1560,7 +1560,7 @@
       <c r="U12" s="13"/>
       <c r="W12">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="W13">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1652,7 +1652,7 @@
       </c>
       <c r="W14">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1692,7 +1692,7 @@
       </c>
       <c r="W15">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="W16">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="W17">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="W18">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -1864,7 +1864,7 @@
       </c>
       <c r="W19">
         <f t="shared" si="6"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="W20">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="W21">
         <f t="shared" si="6"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="28.2" customHeight="1" thickBot="1">
@@ -2002,7 +2002,7 @@
       </c>
       <c r="W22">
         <f t="shared" si="6"/>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="43.2" customHeight="1">
@@ -2038,6 +2038,14 @@
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
+      <c r="V23">
+        <f t="shared" ref="V23:V25" si="9">O23+R23+S23+T23+U23</f>
+        <v>13</v>
+      </c>
+      <c r="W23">
+        <f t="shared" ref="W23:W25" si="10">_xlfn.RANK.EQ(V23, $V$2:$V$1000, 0)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:23" ht="28.8" customHeight="1">
       <c r="A24" s="14">
@@ -2072,6 +2080,14 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
+      <c r="V24">
+        <f t="shared" si="9"/>
+        <v>28.5</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:23" ht="43.2" customHeight="1">
       <c r="A25" s="14">
@@ -2104,6 +2120,14 @@
       </c>
       <c r="Q25">
         <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="9"/>
+        <v>10.75</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
     </row>
@@ -2539,7 +2563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AT17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>

</xml_diff>